<commit_message>
Refine Teacher availability or preferred timeslots and implement  other minor improvements (UI, update logic, etc.)
</commit_message>
<xml_diff>
--- a/import-examples/timetable_data.xlsx
+++ b/import-examples/timetable_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diallofrancispatrick/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52BBC5E-726F-B54D-BD16-7838DECEAE31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5CE883D-87FB-174D-BBDB-DA3159692CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16260" activeTab="2" xr2:uid="{463DB273-5E57-1240-BC5F-E8CC45185236}"/>
   </bookViews>
@@ -79,15 +79,9 @@
     <t>Room C</t>
   </si>
   <si>
-    <t>availableTimeslots</t>
-  </si>
-  <si>
     <t>A. Turing</t>
   </si>
   <si>
-    <t>1,2,4,5</t>
-  </si>
-  <si>
     <t>M. Curie</t>
   </si>
   <si>
@@ -163,7 +157,13 @@
     <t>numberOfStudents</t>
   </si>
   <si>
-    <t>2, 5</t>
+    <t>preferredTimeslots</t>
+  </si>
+  <si>
+    <t>TUESDAY/10:00-16:00|WEDNESDAY/09:00-15:00</t>
+  </si>
+  <si>
+    <t>MONDAY/08:00-12:00</t>
   </si>
 </sst>
 </file>
@@ -210,14 +210,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -711,12 +710,12 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="3" max="3" width="41" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -727,7 +726,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -735,10 +734,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -746,7 +745,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -754,10 +753,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>40</v>
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -785,19 +784,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -805,16 +804,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" t="s">
-        <v>23</v>
       </c>
       <c r="F2">
         <v>15</v>
@@ -846,22 +845,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -869,7 +868,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -878,10 +877,10 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -892,7 +891,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -901,10 +900,10 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -915,7 +914,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -924,10 +923,10 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -938,7 +937,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -947,10 +946,10 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -977,15 +976,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -993,26 +992,26 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement Lesson pinning feature
</commit_message>
<xml_diff>
--- a/import-examples/timetable_data.xlsx
+++ b/import-examples/timetable_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diallofrancispatrick/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diallofrancispatrick/Desktop/workspace/Automatic-Timetable-Generation-System/import-examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5CE883D-87FB-174D-BBDB-DA3159692CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81886E9B-10E5-0C4D-AFAF-2FB8F89CAF08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16260" activeTab="2" xr2:uid="{463DB273-5E57-1240-BC5F-E8CC45185236}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16180" activeTab="4" xr2:uid="{463DB273-5E57-1240-BC5F-E8CC45185236}"/>
   </bookViews>
   <sheets>
     <sheet name="Timeslots" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -164,6 +164,15 @@
   </si>
   <si>
     <t>MONDAY/08:00-12:00</t>
+  </si>
+  <si>
+    <t>pinned</t>
+  </si>
+  <si>
+    <t>timeslotId</t>
+  </si>
+  <si>
+    <t>roomId</t>
   </si>
 </sst>
 </file>
@@ -210,13 +219,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -709,7 +719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9352394-1483-FD4A-950F-4D7AF7150E4B}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -826,10 +836,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CBC01F1-606B-AC4B-9826-7C03E429838C}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -840,7 +850,7 @@
     <col min="7" max="7" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -862,8 +872,17 @@
       <c r="G1" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -885,8 +904,11 @@
       <c r="G2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -908,8 +930,11 @@
       <c r="G3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -931,8 +956,11 @@
       <c r="G4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>6</v>
       </c>
@@ -953,6 +981,15 @@
       </c>
       <c r="G5">
         <v>1</v>
+      </c>
+      <c r="H5" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>